<commit_message>
march 29th change part 1
this is part 1 of the big changes coming to this website
</commit_message>
<xml_diff>
--- a/oh boy.xlsx
+++ b/oh boy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PopsicL\Desktop\carshalton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20487A4C-0509-4E39-A777-85CFC80D991F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2449EAA-4893-4B7F-8352-911BF97F2AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="156">
   <si>
     <t>Verbs:</t>
   </si>
@@ -293,9 +293,6 @@
     <t>yo (rus. Ë)</t>
   </si>
   <si>
-    <t>t̪͡s̪</t>
-  </si>
-  <si>
     <t>* - "rj" makes a "rý" or a "ryá" sound. It's used in some words as: lotérja, intérja. If you do know the IPA letter of "rj", please contact me.</t>
   </si>
   <si>
@@ -344,9 +341,6 @@
     <t>nóšča, wašha, léšhta</t>
   </si>
   <si>
-    <t>Example words: nóšče (to ear), wášhe (to wash), léšhte (to fly)</t>
-  </si>
-  <si>
     <t>nóšču, wašhu, léšhtu</t>
   </si>
   <si>
@@ -498,6 +492,18 @@
   </si>
   <si>
     <t>Locative: Rýbčyňýe, mŕkčynýne, pisméňkčynýne</t>
+  </si>
+  <si>
+    <t>t̪͡s̪ / k</t>
+  </si>
+  <si>
+    <t>Example words: nóšče (to eat), wášhe (to wash), léšhte (to fly)</t>
+  </si>
+  <si>
+    <t>Nominative: Nóšče, wášhe, léšhte</t>
+  </si>
+  <si>
+    <t>Noun Cases (for adjectives)</t>
   </si>
 </sst>
 </file>
@@ -1377,6 +1383,237 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1410,9 +1647,6 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1431,9 +1665,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1461,236 +1692,11 @@
     <xf numFmtId="0" fontId="7" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1979,30 +1985,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67:L67"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M52" sqref="M52:V52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="114" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -2016,28 +2022,28 @@
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="V7" s="97" t="s">
+      <c r="V7" s="74" t="s">
         <v>80</v>
       </c>
-      <c r="W7" s="98"/>
-      <c r="X7" s="98"/>
-      <c r="Y7" s="98"/>
-      <c r="Z7" s="98"/>
-      <c r="AA7" s="99"/>
+      <c r="W7" s="75"/>
+      <c r="X7" s="75"/>
+      <c r="Y7" s="75"/>
+      <c r="Z7" s="75"/>
+      <c r="AA7" s="76"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="V8" s="142" t="s">
+      <c r="V8" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="W8" s="143"/>
-      <c r="X8" s="142" t="s">
+      <c r="W8" s="94"/>
+      <c r="X8" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="Y8" s="143"/>
-      <c r="Z8" s="142" t="s">
+      <c r="Y8" s="94"/>
+      <c r="Z8" s="93" t="s">
         <v>58</v>
       </c>
-      <c r="AA8" s="143"/>
+      <c r="AA8" s="94"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="V9" s="17" t="s">
@@ -2091,7 +2097,7 @@
         <v>34</v>
       </c>
       <c r="Y11" s="9" t="s">
-        <v>85</v>
+        <v>152</v>
       </c>
       <c r="Z11" s="23" t="s">
         <v>61</v>
@@ -2101,25 +2107,25 @@
       </c>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="80" t="s">
+      <c r="C12" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="81"/>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="81"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="81"/>
-      <c r="K12" s="81"/>
-      <c r="L12" s="81"/>
-      <c r="M12" s="81"/>
-      <c r="N12" s="81"/>
-      <c r="O12" s="81"/>
-      <c r="P12" s="81"/>
-      <c r="Q12" s="81"/>
-      <c r="R12" s="81"/>
-      <c r="S12" s="82"/>
+      <c r="D12" s="107"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="107"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="107"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="107"/>
+      <c r="K12" s="107"/>
+      <c r="L12" s="107"/>
+      <c r="M12" s="107"/>
+      <c r="N12" s="107"/>
+      <c r="O12" s="107"/>
+      <c r="P12" s="107"/>
+      <c r="Q12" s="107"/>
+      <c r="R12" s="107"/>
+      <c r="S12" s="108"/>
       <c r="V12" s="19" t="s">
         <v>19</v>
       </c>
@@ -2140,25 +2146,25 @@
       </c>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="84" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" s="85"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="86"/>
-      <c r="L13" s="86"/>
-      <c r="M13" s="86"/>
-      <c r="N13" s="86"/>
-      <c r="O13" s="86"/>
-      <c r="P13" s="86"/>
-      <c r="Q13" s="86"/>
-      <c r="R13" s="86"/>
-      <c r="S13" s="87"/>
+      <c r="C13" s="110" t="s">
+        <v>153</v>
+      </c>
+      <c r="D13" s="111"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="112"/>
+      <c r="G13" s="112"/>
+      <c r="H13" s="112"/>
+      <c r="I13" s="112"/>
+      <c r="J13" s="112"/>
+      <c r="K13" s="112"/>
+      <c r="L13" s="112"/>
+      <c r="M13" s="112"/>
+      <c r="N13" s="112"/>
+      <c r="O13" s="112"/>
+      <c r="P13" s="112"/>
+      <c r="Q13" s="112"/>
+      <c r="R13" s="112"/>
+      <c r="S13" s="113"/>
       <c r="V13" s="25" t="s">
         <v>20</v>
       </c>
@@ -2179,35 +2185,35 @@
       </c>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="128" t="s">
+      <c r="C14" s="121" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="129"/>
-      <c r="E14" s="75" t="s">
-        <v>94</v>
-      </c>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="77" t="s">
+      <c r="D14" s="122"/>
+      <c r="E14" s="102" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="103"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
-      <c r="K14" s="77" t="s">
+      <c r="I14" s="104"/>
+      <c r="J14" s="104"/>
+      <c r="K14" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="L14" s="77"/>
-      <c r="M14" s="77"/>
-      <c r="N14" s="77" t="s">
+      <c r="L14" s="104"/>
+      <c r="M14" s="104"/>
+      <c r="N14" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="O14" s="77"/>
-      <c r="P14" s="77"/>
-      <c r="Q14" s="77" t="s">
+      <c r="O14" s="104"/>
+      <c r="P14" s="104"/>
+      <c r="Q14" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="R14" s="77"/>
-      <c r="S14" s="83"/>
+      <c r="R14" s="104"/>
+      <c r="S14" s="109"/>
       <c r="V14" s="19" t="s">
         <v>21</v>
       </c>
@@ -2228,35 +2234,35 @@
       </c>
     </row>
     <row r="15" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="89" t="s">
+      <c r="C15" s="115" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="90"/>
-      <c r="E15" s="78" t="s">
+      <c r="D15" s="116"/>
+      <c r="E15" s="105" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="F15" s="79"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="79" t="s">
+      <c r="I15" s="87"/>
+      <c r="J15" s="87"/>
+      <c r="K15" s="87" t="s">
+        <v>102</v>
+      </c>
+      <c r="L15" s="87"/>
+      <c r="M15" s="87"/>
+      <c r="N15" s="87" t="s">
         <v>103</v>
       </c>
-      <c r="I15" s="79"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="79" t="s">
+      <c r="O15" s="87"/>
+      <c r="P15" s="87"/>
+      <c r="Q15" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="L15" s="79"/>
-      <c r="M15" s="79"/>
-      <c r="N15" s="79" t="s">
-        <v>105</v>
-      </c>
-      <c r="O15" s="79"/>
-      <c r="P15" s="79"/>
-      <c r="Q15" s="79" t="s">
-        <v>106</v>
-      </c>
-      <c r="R15" s="79"/>
-      <c r="S15" s="131"/>
+      <c r="R15" s="87"/>
+      <c r="S15" s="88"/>
       <c r="V15" s="19" t="s">
         <v>23</v>
       </c>
@@ -2277,27 +2283,27 @@
       </c>
     </row>
     <row r="16" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="91"/>
-      <c r="D16" s="92"/>
+      <c r="C16" s="117"/>
+      <c r="D16" s="118"/>
       <c r="E16" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="F16" s="104" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="104"/>
-      <c r="H16" s="104"/>
-      <c r="I16" s="104"/>
-      <c r="J16" s="104"/>
-      <c r="K16" s="104"/>
-      <c r="L16" s="104"/>
-      <c r="M16" s="104"/>
-      <c r="N16" s="104"/>
-      <c r="O16" s="104"/>
-      <c r="P16" s="104"/>
-      <c r="Q16" s="104"/>
-      <c r="R16" s="104"/>
-      <c r="S16" s="105"/>
+        <v>90</v>
+      </c>
+      <c r="F16" s="81" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" s="81"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="81"/>
+      <c r="M16" s="81"/>
+      <c r="N16" s="81"/>
+      <c r="O16" s="81"/>
+      <c r="P16" s="81"/>
+      <c r="Q16" s="81"/>
+      <c r="R16" s="81"/>
+      <c r="S16" s="82"/>
       <c r="V16" s="25" t="s">
         <v>24</v>
       </c>
@@ -2318,27 +2324,27 @@
       </c>
     </row>
     <row r="17" spans="3:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="91"/>
-      <c r="D17" s="92"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="118"/>
       <c r="E17" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="F17" s="106" t="s">
-        <v>108</v>
-      </c>
-      <c r="G17" s="106"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="106"/>
-      <c r="J17" s="106"/>
-      <c r="K17" s="106"/>
-      <c r="L17" s="106"/>
-      <c r="M17" s="106"/>
-      <c r="N17" s="106"/>
-      <c r="O17" s="106"/>
-      <c r="P17" s="106"/>
-      <c r="Q17" s="106"/>
-      <c r="R17" s="106"/>
-      <c r="S17" s="107"/>
+        <v>91</v>
+      </c>
+      <c r="F17" s="83" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" s="83"/>
+      <c r="H17" s="83"/>
+      <c r="I17" s="83"/>
+      <c r="J17" s="83"/>
+      <c r="K17" s="83"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="83"/>
+      <c r="N17" s="83"/>
+      <c r="O17" s="83"/>
+      <c r="P17" s="83"/>
+      <c r="Q17" s="83"/>
+      <c r="R17" s="83"/>
+      <c r="S17" s="84"/>
       <c r="V17" s="19" t="s">
         <v>25</v>
       </c>
@@ -2359,27 +2365,27 @@
       </c>
     </row>
     <row r="18" spans="3:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="93"/>
-      <c r="D18" s="94"/>
+      <c r="C18" s="119"/>
+      <c r="D18" s="120"/>
       <c r="E18" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="F18" s="108" t="s">
-        <v>109</v>
-      </c>
-      <c r="G18" s="108"/>
-      <c r="H18" s="108"/>
-      <c r="I18" s="108"/>
-      <c r="J18" s="108"/>
-      <c r="K18" s="108"/>
-      <c r="L18" s="108"/>
-      <c r="M18" s="108"/>
-      <c r="N18" s="108"/>
-      <c r="O18" s="108"/>
-      <c r="P18" s="108"/>
-      <c r="Q18" s="108"/>
-      <c r="R18" s="108"/>
-      <c r="S18" s="109"/>
+        <v>92</v>
+      </c>
+      <c r="F18" s="85" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="85"/>
+      <c r="H18" s="85"/>
+      <c r="I18" s="85"/>
+      <c r="J18" s="85"/>
+      <c r="K18" s="85"/>
+      <c r="L18" s="85"/>
+      <c r="M18" s="85"/>
+      <c r="N18" s="85"/>
+      <c r="O18" s="85"/>
+      <c r="P18" s="85"/>
+      <c r="Q18" s="85"/>
+      <c r="R18" s="85"/>
+      <c r="S18" s="86"/>
       <c r="V18" s="25" t="s">
         <v>26</v>
       </c>
@@ -2400,39 +2406,39 @@
       </c>
     </row>
     <row r="19" spans="3:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="66" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="132" t="s">
-        <v>100</v>
-      </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57" t="s">
+      <c r="C19" s="141" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="142"/>
+      <c r="E19" s="89" t="s">
         <v>99</v>
       </c>
-      <c r="I19" s="57"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57" t="s">
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="90" t="s">
         <v>98</v>
       </c>
-      <c r="L19" s="57"/>
-      <c r="M19" s="57"/>
-      <c r="N19" s="55" t="s">
+      <c r="I19" s="90"/>
+      <c r="J19" s="90"/>
+      <c r="K19" s="90" t="s">
         <v>97</v>
       </c>
-      <c r="O19" s="55"/>
-      <c r="P19" s="55"/>
-      <c r="Q19" s="55" t="s">
-        <v>110</v>
-      </c>
-      <c r="R19" s="55"/>
-      <c r="S19" s="56"/>
+      <c r="L19" s="90"/>
+      <c r="M19" s="90"/>
+      <c r="N19" s="132" t="s">
+        <v>96</v>
+      </c>
+      <c r="O19" s="132"/>
+      <c r="P19" s="132"/>
+      <c r="Q19" s="132" t="s">
+        <v>108</v>
+      </c>
+      <c r="R19" s="132"/>
+      <c r="S19" s="133"/>
       <c r="V19" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="W19" s="140" t="s">
+      <c r="W19" s="91" t="s">
         <v>30</v>
       </c>
       <c r="X19" s="21" t="s">
@@ -2441,70 +2447,70 @@
       <c r="Y19" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="Z19" s="144" t="s">
-        <v>86</v>
-      </c>
-      <c r="AA19" s="145"/>
+      <c r="Z19" s="95" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA19" s="96"/>
       <c r="AE19" s="29"/>
     </row>
     <row r="20" spans="3:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="68"/>
-      <c r="D20" s="69"/>
+      <c r="C20" s="143"/>
+      <c r="D20" s="144"/>
       <c r="E20" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="F20" s="95" t="s">
-        <v>123</v>
-      </c>
-      <c r="G20" s="95"/>
-      <c r="H20" s="95"/>
-      <c r="I20" s="95"/>
-      <c r="J20" s="95"/>
-      <c r="K20" s="95"/>
-      <c r="L20" s="95"/>
-      <c r="M20" s="95"/>
-      <c r="N20" s="95"/>
-      <c r="O20" s="95"/>
-      <c r="P20" s="95"/>
-      <c r="Q20" s="95"/>
-      <c r="R20" s="95"/>
-      <c r="S20" s="96"/>
+        <v>90</v>
+      </c>
+      <c r="F20" s="149" t="s">
+        <v>121</v>
+      </c>
+      <c r="G20" s="149"/>
+      <c r="H20" s="149"/>
+      <c r="I20" s="149"/>
+      <c r="J20" s="149"/>
+      <c r="K20" s="149"/>
+      <c r="L20" s="149"/>
+      <c r="M20" s="149"/>
+      <c r="N20" s="149"/>
+      <c r="O20" s="149"/>
+      <c r="P20" s="149"/>
+      <c r="Q20" s="149"/>
+      <c r="R20" s="149"/>
+      <c r="S20" s="150"/>
       <c r="V20" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="W20" s="141"/>
+      <c r="W20" s="92"/>
       <c r="X20" s="21" t="s">
         <v>43</v>
       </c>
       <c r="Y20" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="Z20" s="146"/>
-      <c r="AA20" s="147"/>
+      <c r="Z20" s="97"/>
+      <c r="AA20" s="98"/>
       <c r="AE20" s="29"/>
     </row>
     <row r="21" spans="3:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="68"/>
-      <c r="D21" s="69"/>
+      <c r="C21" s="143"/>
+      <c r="D21" s="144"/>
       <c r="E21" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="F21" s="100" t="s">
-        <v>122</v>
-      </c>
-      <c r="G21" s="100"/>
-      <c r="H21" s="100"/>
-      <c r="I21" s="100"/>
-      <c r="J21" s="100"/>
-      <c r="K21" s="100"/>
-      <c r="L21" s="100"/>
-      <c r="M21" s="100"/>
-      <c r="N21" s="100"/>
-      <c r="O21" s="100"/>
-      <c r="P21" s="100"/>
-      <c r="Q21" s="100"/>
-      <c r="R21" s="100"/>
-      <c r="S21" s="101"/>
+        <v>91</v>
+      </c>
+      <c r="F21" s="77" t="s">
+        <v>120</v>
+      </c>
+      <c r="G21" s="77"/>
+      <c r="H21" s="77"/>
+      <c r="I21" s="77"/>
+      <c r="J21" s="77"/>
+      <c r="K21" s="77"/>
+      <c r="L21" s="77"/>
+      <c r="M21" s="77"/>
+      <c r="N21" s="77"/>
+      <c r="O21" s="77"/>
+      <c r="P21" s="77"/>
+      <c r="Q21" s="77"/>
+      <c r="R21" s="77"/>
+      <c r="S21" s="78"/>
       <c r="V21" s="7"/>
       <c r="W21" s="7"/>
       <c r="X21" s="21" t="s">
@@ -2513,234 +2519,234 @@
       <c r="Y21" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="Z21" s="146"/>
-      <c r="AA21" s="147"/>
+      <c r="Z21" s="97"/>
+      <c r="AA21" s="98"/>
       <c r="AE21" s="29"/>
     </row>
     <row r="22" spans="3:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="70"/>
-      <c r="D22" s="71"/>
+      <c r="C22" s="145"/>
+      <c r="D22" s="146"/>
       <c r="E22" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="F22" s="102" t="s">
-        <v>124</v>
-      </c>
-      <c r="G22" s="102"/>
-      <c r="H22" s="102"/>
-      <c r="I22" s="102"/>
-      <c r="J22" s="102"/>
-      <c r="K22" s="102"/>
-      <c r="L22" s="102"/>
-      <c r="M22" s="102"/>
-      <c r="N22" s="102"/>
-      <c r="O22" s="102"/>
-      <c r="P22" s="102"/>
-      <c r="Q22" s="102"/>
-      <c r="R22" s="102"/>
-      <c r="S22" s="103"/>
+        <v>92</v>
+      </c>
+      <c r="F22" s="79" t="s">
+        <v>122</v>
+      </c>
+      <c r="G22" s="79"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="79"/>
+      <c r="J22" s="79"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="79"/>
+      <c r="M22" s="79"/>
+      <c r="N22" s="79"/>
+      <c r="O22" s="79"/>
+      <c r="P22" s="79"/>
+      <c r="Q22" s="79"/>
+      <c r="R22" s="79"/>
+      <c r="S22" s="80"/>
       <c r="X22" s="27" t="s">
         <v>45</v>
       </c>
       <c r="Y22" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="Z22" s="146"/>
-      <c r="AA22" s="147"/>
+        <v>119</v>
+      </c>
+      <c r="Z22" s="97"/>
+      <c r="AA22" s="98"/>
     </row>
     <row r="23" spans="3:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="114" t="s">
+      <c r="C23" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="115"/>
-      <c r="E23" s="133" t="s">
+      <c r="D23" s="52"/>
+      <c r="E23" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68" t="s">
+        <v>110</v>
+      </c>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="68" t="s">
         <v>111</v>
       </c>
-      <c r="F23" s="134"/>
-      <c r="G23" s="134"/>
-      <c r="H23" s="134" t="s">
+      <c r="L23" s="68"/>
+      <c r="M23" s="68"/>
+      <c r="N23" s="68" t="s">
         <v>112</v>
       </c>
-      <c r="I23" s="134"/>
-      <c r="J23" s="134"/>
-      <c r="K23" s="134" t="s">
+      <c r="O23" s="68"/>
+      <c r="P23" s="68"/>
+      <c r="Q23" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="L23" s="134"/>
-      <c r="M23" s="134"/>
-      <c r="N23" s="134" t="s">
-        <v>114</v>
-      </c>
-      <c r="O23" s="134"/>
-      <c r="P23" s="134"/>
-      <c r="Q23" s="134" t="s">
-        <v>115</v>
-      </c>
-      <c r="R23" s="134"/>
-      <c r="S23" s="135"/>
+      <c r="R23" s="68"/>
+      <c r="S23" s="69"/>
       <c r="X23" s="21" t="s">
         <v>46</v>
       </c>
       <c r="Y23" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="Z23" s="146"/>
-      <c r="AA23" s="147"/>
+      <c r="Z23" s="97"/>
+      <c r="AA23" s="98"/>
     </row>
     <row r="24" spans="3:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="116"/>
-      <c r="D24" s="117"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="54"/>
       <c r="E24" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="F24" s="126" t="s">
-        <v>127</v>
-      </c>
-      <c r="G24" s="126"/>
-      <c r="H24" s="126"/>
-      <c r="I24" s="126"/>
-      <c r="J24" s="126"/>
-      <c r="K24" s="126"/>
-      <c r="L24" s="126"/>
-      <c r="M24" s="126"/>
-      <c r="N24" s="126"/>
-      <c r="O24" s="126"/>
-      <c r="P24" s="126"/>
-      <c r="Q24" s="126"/>
-      <c r="R24" s="126"/>
-      <c r="S24" s="127"/>
+        <v>90</v>
+      </c>
+      <c r="F24" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="G24" s="63"/>
+      <c r="H24" s="63"/>
+      <c r="I24" s="63"/>
+      <c r="J24" s="63"/>
+      <c r="K24" s="63"/>
+      <c r="L24" s="63"/>
+      <c r="M24" s="63"/>
+      <c r="N24" s="63"/>
+      <c r="O24" s="63"/>
+      <c r="P24" s="63"/>
+      <c r="Q24" s="63"/>
+      <c r="R24" s="63"/>
+      <c r="S24" s="64"/>
       <c r="X24" s="21" t="s">
         <v>47</v>
       </c>
       <c r="Y24" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="Z24" s="146"/>
-      <c r="AA24" s="147"/>
+      <c r="Z24" s="97"/>
+      <c r="AA24" s="98"/>
     </row>
     <row r="25" spans="3:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="116"/>
-      <c r="D25" s="117"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="54"/>
       <c r="E25" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="F25" s="136" t="s">
-        <v>126</v>
-      </c>
-      <c r="G25" s="136"/>
-      <c r="H25" s="136"/>
-      <c r="I25" s="136"/>
-      <c r="J25" s="136"/>
-      <c r="K25" s="136"/>
-      <c r="L25" s="136"/>
-      <c r="M25" s="136"/>
-      <c r="N25" s="136"/>
-      <c r="O25" s="136"/>
-      <c r="P25" s="136"/>
-      <c r="Q25" s="136"/>
-      <c r="R25" s="136"/>
-      <c r="S25" s="137"/>
+        <v>91</v>
+      </c>
+      <c r="F25" s="70" t="s">
+        <v>124</v>
+      </c>
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="70"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="70"/>
+      <c r="L25" s="70"/>
+      <c r="M25" s="70"/>
+      <c r="N25" s="70"/>
+      <c r="O25" s="70"/>
+      <c r="P25" s="70"/>
+      <c r="Q25" s="70"/>
+      <c r="R25" s="70"/>
+      <c r="S25" s="71"/>
       <c r="X25" s="27" t="s">
         <v>48</v>
       </c>
       <c r="Y25" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="Z25" s="146"/>
-      <c r="AA25" s="147"/>
+      <c r="Z25" s="97"/>
+      <c r="AA25" s="98"/>
     </row>
     <row r="26" spans="3:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="118"/>
-      <c r="D26" s="119"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="56"/>
       <c r="E26" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="F26" s="138" t="s">
-        <v>125</v>
-      </c>
-      <c r="G26" s="138"/>
-      <c r="H26" s="138"/>
-      <c r="I26" s="138"/>
-      <c r="J26" s="138"/>
-      <c r="K26" s="138"/>
-      <c r="L26" s="138"/>
-      <c r="M26" s="138"/>
-      <c r="N26" s="138"/>
-      <c r="O26" s="138"/>
-      <c r="P26" s="138"/>
-      <c r="Q26" s="138"/>
-      <c r="R26" s="138"/>
-      <c r="S26" s="139"/>
+        <v>92</v>
+      </c>
+      <c r="F26" s="72" t="s">
+        <v>123</v>
+      </c>
+      <c r="G26" s="72"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="72"/>
+      <c r="J26" s="72"/>
+      <c r="K26" s="72"/>
+      <c r="L26" s="72"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="72"/>
+      <c r="O26" s="72"/>
+      <c r="P26" s="72"/>
+      <c r="Q26" s="72"/>
+      <c r="R26" s="72"/>
+      <c r="S26" s="73"/>
       <c r="X26" s="21" t="s">
         <v>49</v>
       </c>
       <c r="Y26" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="Z26" s="146"/>
-      <c r="AA26" s="147"/>
+      <c r="Z26" s="97"/>
+      <c r="AA26" s="98"/>
     </row>
     <row r="27" spans="3:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="120" t="s">
+      <c r="C27" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="D27" s="121"/>
-      <c r="E27" s="130" t="s">
+      <c r="D27" s="58"/>
+      <c r="E27" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66" t="s">
+        <v>115</v>
+      </c>
+      <c r="I27" s="66"/>
+      <c r="J27" s="66"/>
+      <c r="K27" s="66" t="s">
         <v>116</v>
       </c>
-      <c r="F27" s="64"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="64" t="s">
+      <c r="L27" s="66"/>
+      <c r="M27" s="66"/>
+      <c r="N27" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="I27" s="64"/>
-      <c r="J27" s="64"/>
-      <c r="K27" s="64" t="s">
+      <c r="O27" s="66"/>
+      <c r="P27" s="66"/>
+      <c r="Q27" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="L27" s="64"/>
-      <c r="M27" s="64"/>
-      <c r="N27" s="64" t="s">
-        <v>119</v>
-      </c>
-      <c r="O27" s="64"/>
-      <c r="P27" s="64"/>
-      <c r="Q27" s="64" t="s">
-        <v>120</v>
-      </c>
-      <c r="R27" s="64"/>
-      <c r="S27" s="65"/>
+      <c r="R27" s="66"/>
+      <c r="S27" s="140"/>
       <c r="X27" s="27" t="s">
         <v>50</v>
       </c>
       <c r="Y27" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="Z27" s="148"/>
-      <c r="AA27" s="149"/>
+      <c r="Z27" s="99"/>
+      <c r="AA27" s="100"/>
     </row>
     <row r="28" spans="3:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="122"/>
-      <c r="D28" s="123"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="60"/>
       <c r="E28" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="F28" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="G28" s="72"/>
-      <c r="H28" s="72"/>
-      <c r="I28" s="72"/>
-      <c r="J28" s="72"/>
-      <c r="K28" s="72"/>
-      <c r="L28" s="72"/>
-      <c r="M28" s="72"/>
-      <c r="N28" s="72"/>
-      <c r="O28" s="72"/>
-      <c r="P28" s="72"/>
-      <c r="Q28" s="72"/>
-      <c r="R28" s="72"/>
-      <c r="S28" s="73"/>
+        <v>90</v>
+      </c>
+      <c r="F28" s="147" t="s">
+        <v>126</v>
+      </c>
+      <c r="G28" s="147"/>
+      <c r="H28" s="147"/>
+      <c r="I28" s="147"/>
+      <c r="J28" s="147"/>
+      <c r="K28" s="147"/>
+      <c r="L28" s="147"/>
+      <c r="M28" s="147"/>
+      <c r="N28" s="147"/>
+      <c r="O28" s="147"/>
+      <c r="P28" s="147"/>
+      <c r="Q28" s="147"/>
+      <c r="R28" s="147"/>
+      <c r="S28" s="148"/>
       <c r="X28" s="21" t="s">
         <v>51</v>
       </c>
@@ -2749,27 +2755,27 @@
       </c>
     </row>
     <row r="29" spans="3:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="122"/>
-      <c r="D29" s="123"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="60"/>
       <c r="E29" s="43" t="s">
-        <v>92</v>
-      </c>
-      <c r="F29" s="110" t="s">
-        <v>129</v>
-      </c>
-      <c r="G29" s="110"/>
-      <c r="H29" s="110"/>
-      <c r="I29" s="110"/>
-      <c r="J29" s="110"/>
-      <c r="K29" s="110"/>
-      <c r="L29" s="110"/>
-      <c r="M29" s="110"/>
-      <c r="N29" s="110"/>
-      <c r="O29" s="110"/>
-      <c r="P29" s="110"/>
-      <c r="Q29" s="110"/>
-      <c r="R29" s="110"/>
-      <c r="S29" s="111"/>
+        <v>91</v>
+      </c>
+      <c r="F29" s="47" t="s">
+        <v>127</v>
+      </c>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="47"/>
+      <c r="P29" s="47"/>
+      <c r="Q29" s="47"/>
+      <c r="R29" s="47"/>
+      <c r="S29" s="48"/>
       <c r="X29" s="21" t="s">
         <v>52</v>
       </c>
@@ -2778,27 +2784,27 @@
       </c>
     </row>
     <row r="30" spans="3:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="124"/>
-      <c r="D30" s="125"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="62"/>
       <c r="E30" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="F30" s="112" t="s">
-        <v>130</v>
-      </c>
-      <c r="G30" s="112"/>
-      <c r="H30" s="112"/>
-      <c r="I30" s="112"/>
-      <c r="J30" s="112"/>
-      <c r="K30" s="112"/>
-      <c r="L30" s="112"/>
-      <c r="M30" s="112"/>
-      <c r="N30" s="112"/>
-      <c r="O30" s="112"/>
-      <c r="P30" s="112"/>
-      <c r="Q30" s="112"/>
-      <c r="R30" s="112"/>
-      <c r="S30" s="113"/>
+        <v>92</v>
+      </c>
+      <c r="F30" s="49" t="s">
+        <v>128</v>
+      </c>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="49"/>
+      <c r="O30" s="49"/>
+      <c r="P30" s="49"/>
+      <c r="Q30" s="49"/>
+      <c r="R30" s="49"/>
+      <c r="S30" s="50"/>
       <c r="X30" s="21" t="s">
         <v>53</v>
       </c>
@@ -2807,25 +2813,25 @@
       </c>
     </row>
     <row r="31" spans="3:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
-      <c r="K31" s="47"/>
-      <c r="L31" s="47"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="47"/>
-      <c r="O31" s="47"/>
-      <c r="P31" s="47"/>
-      <c r="Q31" s="47"/>
-      <c r="R31" s="47"/>
-      <c r="S31" s="48"/>
+      <c r="C31" s="123" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="124"/>
+      <c r="E31" s="124"/>
+      <c r="F31" s="124"/>
+      <c r="G31" s="124"/>
+      <c r="H31" s="124"/>
+      <c r="I31" s="124"/>
+      <c r="J31" s="124"/>
+      <c r="K31" s="124"/>
+      <c r="L31" s="124"/>
+      <c r="M31" s="124"/>
+      <c r="N31" s="124"/>
+      <c r="O31" s="124"/>
+      <c r="P31" s="124"/>
+      <c r="Q31" s="124"/>
+      <c r="R31" s="124"/>
+      <c r="S31" s="125"/>
       <c r="X31" s="21" t="s">
         <v>54</v>
       </c>
@@ -2860,40 +2866,40 @@
     </row>
     <row r="35" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="61" t="s">
+      <c r="C36" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="62"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="62"/>
-      <c r="G36" s="63"/>
+      <c r="D36" s="138"/>
+      <c r="E36" s="138"/>
+      <c r="F36" s="138"/>
+      <c r="G36" s="139"/>
     </row>
     <row r="37" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="58" t="s">
+      <c r="C37" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="59"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="60"/>
+      <c r="D37" s="135"/>
+      <c r="E37" s="135"/>
+      <c r="F37" s="135"/>
+      <c r="G37" s="136"/>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="49" t="s">
+      <c r="C38" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="50"/>
-      <c r="G38" s="51"/>
+      <c r="D38" s="127"/>
+      <c r="E38" s="127"/>
+      <c r="F38" s="127"/>
+      <c r="G38" s="128"/>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="52" t="s">
+      <c r="C39" s="129" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="53"/>
-      <c r="G39" s="54"/>
+      <c r="D39" s="130"/>
+      <c r="E39" s="130"/>
+      <c r="F39" s="130"/>
+      <c r="G39" s="131"/>
     </row>
     <row r="40" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="1" t="s">
@@ -2906,328 +2912,493 @@
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C52" s="150" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C52" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="D52" s="46"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="46"/>
+      <c r="G52" s="46"/>
+      <c r="H52" s="46"/>
+      <c r="I52" s="46"/>
+      <c r="J52" s="46"/>
+      <c r="K52" s="46"/>
+      <c r="L52" s="46"/>
+      <c r="M52" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="N52" s="46"/>
+      <c r="O52" s="46"/>
+      <c r="P52" s="46"/>
+      <c r="Q52" s="46"/>
+      <c r="R52" s="46"/>
+      <c r="S52" s="46"/>
+      <c r="T52" s="46"/>
+      <c r="U52" s="46"/>
+      <c r="V52" s="46"/>
+    </row>
+    <row r="53" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C53" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" s="46"/>
+      <c r="E53" s="46"/>
+      <c r="F53" s="46"/>
+      <c r="G53" s="46"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="46"/>
+      <c r="J53" s="46"/>
+      <c r="K53" s="46"/>
+      <c r="L53" s="46"/>
+      <c r="M53" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="N53" s="46"/>
+      <c r="O53" s="46"/>
+      <c r="P53" s="46"/>
+      <c r="Q53" s="46"/>
+      <c r="R53" s="46"/>
+      <c r="S53" s="46"/>
+      <c r="T53" s="46"/>
+      <c r="U53" s="46"/>
+      <c r="V53" s="46"/>
+    </row>
+    <row r="54" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C54" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="D54" s="46"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="I54" s="46"/>
+      <c r="J54" s="46"/>
+      <c r="K54" s="46"/>
+      <c r="L54" s="46"/>
+      <c r="M54" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="N54" s="46"/>
+      <c r="O54" s="46"/>
+      <c r="P54" s="46"/>
+      <c r="Q54" s="46"/>
+      <c r="R54" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="S54" s="46"/>
+      <c r="T54" s="46"/>
+      <c r="U54" s="46"/>
+      <c r="V54" s="46"/>
+    </row>
+    <row r="55" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C55" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="D52" s="150"/>
-      <c r="E52" s="150"/>
-      <c r="F52" s="150"/>
-      <c r="G52" s="150"/>
-      <c r="H52" s="150"/>
-      <c r="I52" s="150"/>
-      <c r="J52" s="150"/>
-      <c r="K52" s="150"/>
-      <c r="L52" s="150"/>
-    </row>
-    <row r="53" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C53" s="150" t="s">
+      <c r="D55" s="46"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="46"/>
+      <c r="H55" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="I55" s="46"/>
+      <c r="J55" s="46"/>
+      <c r="K55" s="46"/>
+      <c r="L55" s="46"/>
+      <c r="M55" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="N55" s="46"/>
+      <c r="O55" s="46"/>
+      <c r="P55" s="46"/>
+      <c r="Q55" s="46"/>
+      <c r="R55" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="S55" s="46"/>
+      <c r="T55" s="46"/>
+      <c r="U55" s="46"/>
+      <c r="V55" s="46"/>
+    </row>
+    <row r="56" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C56" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="D53" s="150"/>
-      <c r="E53" s="150"/>
-      <c r="F53" s="150"/>
-      <c r="G53" s="150"/>
-      <c r="H53" s="150"/>
-      <c r="I53" s="150"/>
-      <c r="J53" s="150"/>
-      <c r="K53" s="150"/>
-      <c r="L53" s="150"/>
-    </row>
-    <row r="54" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C54" s="150" t="s">
-        <v>131</v>
-      </c>
-      <c r="D54" s="150"/>
-      <c r="E54" s="150"/>
-      <c r="F54" s="150"/>
-      <c r="G54" s="150"/>
-      <c r="H54" s="150" t="s">
+      <c r="D56" s="46"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="46"/>
+      <c r="G56" s="46"/>
+      <c r="H56" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="I54" s="150"/>
-      <c r="J54" s="150"/>
-      <c r="K54" s="150"/>
-      <c r="L54" s="150"/>
-    </row>
-    <row r="55" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C55" s="150" t="s">
+      <c r="I56" s="46"/>
+      <c r="J56" s="46"/>
+      <c r="K56" s="46"/>
+      <c r="L56" s="46"/>
+      <c r="M56" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="N56" s="46"/>
+      <c r="O56" s="46"/>
+      <c r="P56" s="46"/>
+      <c r="Q56" s="46"/>
+      <c r="R56" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="S56" s="46"/>
+      <c r="T56" s="46"/>
+      <c r="U56" s="46"/>
+      <c r="V56" s="46"/>
+    </row>
+    <row r="57" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C57" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="D55" s="150"/>
-      <c r="E55" s="150"/>
-      <c r="F55" s="150"/>
-      <c r="G55" s="150"/>
-      <c r="H55" s="150" t="s">
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="I55" s="150"/>
-      <c r="J55" s="150"/>
-      <c r="K55" s="150"/>
-      <c r="L55" s="150"/>
-    </row>
-    <row r="56" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C56" s="150" t="s">
+      <c r="I57" s="46"/>
+      <c r="J57" s="46"/>
+      <c r="K57" s="46"/>
+      <c r="L57" s="46"/>
+      <c r="M57" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="N57" s="46"/>
+      <c r="O57" s="46"/>
+      <c r="P57" s="46"/>
+      <c r="Q57" s="46"/>
+      <c r="R57" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="S57" s="46"/>
+      <c r="T57" s="46"/>
+      <c r="U57" s="46"/>
+      <c r="V57" s="46"/>
+    </row>
+    <row r="58" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C58" s="46" t="s">
         <v>135</v>
       </c>
-      <c r="D56" s="150"/>
-      <c r="E56" s="150"/>
-      <c r="F56" s="150"/>
-      <c r="G56" s="150"/>
-      <c r="H56" s="150" t="s">
+      <c r="D58" s="46"/>
+      <c r="E58" s="46"/>
+      <c r="F58" s="46"/>
+      <c r="G58" s="46"/>
+      <c r="H58" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="I56" s="150"/>
-      <c r="J56" s="150"/>
-      <c r="K56" s="150"/>
-      <c r="L56" s="150"/>
-    </row>
-    <row r="57" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C57" s="150" t="s">
+      <c r="I58" s="46"/>
+      <c r="J58" s="46"/>
+      <c r="K58" s="46"/>
+      <c r="L58" s="46"/>
+      <c r="M58" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="N58" s="46"/>
+      <c r="O58" s="46"/>
+      <c r="P58" s="46"/>
+      <c r="Q58" s="46"/>
+      <c r="R58" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="S58" s="46"/>
+      <c r="T58" s="46"/>
+      <c r="U58" s="46"/>
+      <c r="V58" s="46"/>
+    </row>
+    <row r="59" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C59" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="D59" s="46"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="46"/>
+      <c r="H59" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="I59" s="46"/>
+      <c r="J59" s="46"/>
+      <c r="K59" s="46"/>
+      <c r="L59" s="46"/>
+      <c r="M59" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="N59" s="46"/>
+      <c r="O59" s="46"/>
+      <c r="P59" s="46"/>
+      <c r="Q59" s="46"/>
+      <c r="R59" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="S59" s="46"/>
+      <c r="T59" s="46"/>
+      <c r="U59" s="46"/>
+      <c r="V59" s="46"/>
+    </row>
+    <row r="60" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C60" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="D57" s="150"/>
-      <c r="E57" s="150"/>
-      <c r="F57" s="150"/>
-      <c r="G57" s="150"/>
-      <c r="H57" s="150" t="s">
-        <v>149</v>
-      </c>
-      <c r="I57" s="150"/>
-      <c r="J57" s="150"/>
-      <c r="K57" s="150"/>
-      <c r="L57" s="150"/>
-    </row>
-    <row r="58" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C58" s="150" t="s">
+      <c r="D60" s="46"/>
+      <c r="E60" s="46"/>
+      <c r="F60" s="46"/>
+      <c r="G60" s="46"/>
+      <c r="H60" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="I60" s="46"/>
+      <c r="J60" s="46"/>
+      <c r="K60" s="46"/>
+      <c r="L60" s="46"/>
+      <c r="M60" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="N60" s="46"/>
+      <c r="O60" s="46"/>
+      <c r="P60" s="46"/>
+      <c r="Q60" s="46"/>
+      <c r="R60" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="S60" s="46"/>
+      <c r="T60" s="46"/>
+      <c r="U60" s="46"/>
+      <c r="V60" s="46"/>
+    </row>
+    <row r="61" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C61" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="D58" s="150"/>
-      <c r="E58" s="150"/>
-      <c r="F58" s="150"/>
-      <c r="G58" s="150"/>
-      <c r="H58" s="150" t="s">
-        <v>150</v>
-      </c>
-      <c r="I58" s="150"/>
-      <c r="J58" s="150"/>
-      <c r="K58" s="150"/>
-      <c r="L58" s="150"/>
-    </row>
-    <row r="59" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C59" s="150" t="s">
-        <v>151</v>
-      </c>
-      <c r="D59" s="150"/>
-      <c r="E59" s="150"/>
-      <c r="F59" s="150"/>
-      <c r="G59" s="150"/>
-      <c r="H59" s="150" t="s">
-        <v>153</v>
-      </c>
-      <c r="I59" s="150"/>
-      <c r="J59" s="150"/>
-      <c r="K59" s="150"/>
-      <c r="L59" s="150"/>
-    </row>
-    <row r="60" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C60" s="150" t="s">
+      <c r="D61" s="46"/>
+      <c r="E61" s="46"/>
+      <c r="F61" s="46"/>
+      <c r="G61" s="46"/>
+      <c r="H61" s="46"/>
+      <c r="I61" s="46"/>
+      <c r="J61" s="46"/>
+      <c r="K61" s="46"/>
+      <c r="L61" s="46"/>
+      <c r="M61" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="N61" s="46"/>
+      <c r="O61" s="46"/>
+      <c r="P61" s="46"/>
+      <c r="Q61" s="46"/>
+      <c r="R61" s="46"/>
+      <c r="S61" s="46"/>
+      <c r="T61" s="46"/>
+      <c r="U61" s="46"/>
+      <c r="V61" s="46"/>
+    </row>
+    <row r="62" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C62" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="D62" s="46"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="46"/>
+      <c r="G62" s="46"/>
+      <c r="H62" s="46"/>
+      <c r="I62" s="46"/>
+      <c r="J62" s="46"/>
+      <c r="K62" s="46"/>
+      <c r="L62" s="46"/>
+      <c r="M62" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="N62" s="46"/>
+      <c r="O62" s="46"/>
+      <c r="P62" s="46"/>
+      <c r="Q62" s="46"/>
+      <c r="R62" s="46"/>
+      <c r="S62" s="46"/>
+      <c r="T62" s="46"/>
+      <c r="U62" s="46"/>
+      <c r="V62" s="46"/>
+    </row>
+    <row r="63" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C63" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="D63" s="46"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="46"/>
+      <c r="G63" s="46"/>
+      <c r="H63" s="46"/>
+      <c r="I63" s="46"/>
+      <c r="J63" s="46"/>
+      <c r="K63" s="46"/>
+      <c r="L63" s="46"/>
+      <c r="M63" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="N63" s="46"/>
+      <c r="O63" s="46"/>
+      <c r="P63" s="46"/>
+      <c r="Q63" s="46"/>
+      <c r="R63" s="46"/>
+      <c r="S63" s="46"/>
+      <c r="T63" s="46"/>
+      <c r="U63" s="46"/>
+      <c r="V63" s="46"/>
+    </row>
+    <row r="64" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C64" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="D64" s="46"/>
+      <c r="E64" s="46"/>
+      <c r="F64" s="46"/>
+      <c r="G64" s="46"/>
+      <c r="H64" s="46"/>
+      <c r="I64" s="46"/>
+      <c r="J64" s="46"/>
+      <c r="K64" s="46"/>
+      <c r="L64" s="46"/>
+      <c r="M64" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="N64" s="46"/>
+      <c r="O64" s="46"/>
+      <c r="P64" s="46"/>
+      <c r="Q64" s="46"/>
+      <c r="R64" s="46"/>
+      <c r="S64" s="46"/>
+      <c r="T64" s="46"/>
+      <c r="U64" s="46"/>
+      <c r="V64" s="46"/>
+    </row>
+    <row r="65" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C65" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="D60" s="150"/>
-      <c r="E60" s="150"/>
-      <c r="F60" s="150"/>
-      <c r="G60" s="150"/>
-      <c r="H60" s="150" t="s">
-        <v>152</v>
-      </c>
-      <c r="I60" s="150"/>
-      <c r="J60" s="150"/>
-      <c r="K60" s="150"/>
-      <c r="L60" s="150"/>
-    </row>
-    <row r="61" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C61" s="150" t="s">
-        <v>139</v>
-      </c>
-      <c r="D61" s="150"/>
-      <c r="E61" s="150"/>
-      <c r="F61" s="150"/>
-      <c r="G61" s="150"/>
-      <c r="H61" s="150"/>
-      <c r="I61" s="150"/>
-      <c r="J61" s="150"/>
-      <c r="K61" s="150"/>
-      <c r="L61" s="150"/>
-    </row>
-    <row r="62" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C62" s="150" t="s">
-        <v>144</v>
-      </c>
-      <c r="D62" s="150"/>
-      <c r="E62" s="150"/>
-      <c r="F62" s="150"/>
-      <c r="G62" s="150"/>
-      <c r="H62" s="150"/>
-      <c r="I62" s="150"/>
-      <c r="J62" s="150"/>
-      <c r="K62" s="150"/>
-      <c r="L62" s="150"/>
-    </row>
-    <row r="63" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C63" s="150" t="s">
+      <c r="D65" s="46"/>
+      <c r="E65" s="46"/>
+      <c r="F65" s="46"/>
+      <c r="G65" s="46"/>
+      <c r="H65" s="46"/>
+      <c r="I65" s="46"/>
+      <c r="J65" s="46"/>
+      <c r="K65" s="46"/>
+      <c r="L65" s="46"/>
+      <c r="M65" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="N65" s="46"/>
+      <c r="O65" s="46"/>
+      <c r="P65" s="46"/>
+      <c r="Q65" s="46"/>
+      <c r="R65" s="46"/>
+      <c r="S65" s="46"/>
+      <c r="T65" s="46"/>
+      <c r="U65" s="46"/>
+      <c r="V65" s="46"/>
+    </row>
+    <row r="66" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C66" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="46"/>
+      <c r="I66" s="46"/>
+      <c r="J66" s="46"/>
+      <c r="K66" s="46"/>
+      <c r="L66" s="46"/>
+      <c r="M66" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="N66" s="46"/>
+      <c r="O66" s="46"/>
+      <c r="P66" s="46"/>
+      <c r="Q66" s="46"/>
+      <c r="R66" s="46"/>
+      <c r="S66" s="46"/>
+      <c r="T66" s="46"/>
+      <c r="U66" s="46"/>
+      <c r="V66" s="46"/>
+    </row>
+    <row r="67" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C67" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="D63" s="150"/>
-      <c r="E63" s="150"/>
-      <c r="F63" s="150"/>
-      <c r="G63" s="150"/>
-      <c r="H63" s="150"/>
-      <c r="I63" s="150"/>
-      <c r="J63" s="150"/>
-      <c r="K63" s="150"/>
-      <c r="L63" s="150"/>
-    </row>
-    <row r="64" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C64" s="150" t="s">
-        <v>145</v>
-      </c>
-      <c r="D64" s="150"/>
-      <c r="E64" s="150"/>
-      <c r="F64" s="150"/>
-      <c r="G64" s="150"/>
-      <c r="H64" s="150"/>
-      <c r="I64" s="150"/>
-      <c r="J64" s="150"/>
-      <c r="K64" s="150"/>
-      <c r="L64" s="150"/>
-    </row>
-    <row r="65" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C65" s="150" t="s">
-        <v>140</v>
-      </c>
-      <c r="D65" s="150"/>
-      <c r="E65" s="150"/>
-      <c r="F65" s="150"/>
-      <c r="G65" s="150"/>
-      <c r="H65" s="150"/>
-      <c r="I65" s="150"/>
-      <c r="J65" s="150"/>
-      <c r="K65" s="150"/>
-      <c r="L65" s="150"/>
-    </row>
-    <row r="66" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C66" s="150" t="s">
-        <v>142</v>
-      </c>
-      <c r="D66" s="150"/>
-      <c r="E66" s="150"/>
-      <c r="F66" s="150"/>
-      <c r="G66" s="150"/>
-      <c r="H66" s="150"/>
-      <c r="I66" s="150"/>
-      <c r="J66" s="150"/>
-      <c r="K66" s="150"/>
-      <c r="L66" s="150"/>
-    </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C67" s="150" t="s">
-        <v>143</v>
-      </c>
-      <c r="D67" s="150"/>
-      <c r="E67" s="150"/>
-      <c r="F67" s="150"/>
-      <c r="G67" s="150"/>
-      <c r="H67" s="150"/>
-      <c r="I67" s="150"/>
-      <c r="J67" s="150"/>
-      <c r="K67" s="150"/>
-      <c r="L67" s="150"/>
+      <c r="D67" s="46"/>
+      <c r="E67" s="46"/>
+      <c r="F67" s="46"/>
+      <c r="G67" s="46"/>
+      <c r="H67" s="46"/>
+      <c r="I67" s="46"/>
+      <c r="J67" s="46"/>
+      <c r="K67" s="46"/>
+      <c r="L67" s="46"/>
+      <c r="M67" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="N67" s="46"/>
+      <c r="O67" s="46"/>
+      <c r="P67" s="46"/>
+      <c r="Q67" s="46"/>
+      <c r="R67" s="46"/>
+      <c r="S67" s="46"/>
+      <c r="T67" s="46"/>
+      <c r="U67" s="46"/>
+      <c r="V67" s="46"/>
     </row>
   </sheetData>
-  <mergeCells count="80">
-    <mergeCell ref="C52:L52"/>
-    <mergeCell ref="C53:L53"/>
-    <mergeCell ref="C61:L61"/>
-    <mergeCell ref="C62:L62"/>
-    <mergeCell ref="C63:L63"/>
-    <mergeCell ref="C64:L64"/>
-    <mergeCell ref="C65:L65"/>
-    <mergeCell ref="C66:L66"/>
-    <mergeCell ref="C67:L67"/>
-    <mergeCell ref="C59:G59"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="H54:L54"/>
-    <mergeCell ref="H55:L55"/>
-    <mergeCell ref="H56:L56"/>
-    <mergeCell ref="H57:L57"/>
-    <mergeCell ref="H58:L58"/>
-    <mergeCell ref="H59:L59"/>
-    <mergeCell ref="H60:L60"/>
-    <mergeCell ref="C54:G54"/>
-    <mergeCell ref="C55:G55"/>
-    <mergeCell ref="C56:G56"/>
-    <mergeCell ref="C57:G57"/>
-    <mergeCell ref="C58:G58"/>
-    <mergeCell ref="F29:S29"/>
-    <mergeCell ref="F30:S30"/>
-    <mergeCell ref="C23:D26"/>
-    <mergeCell ref="C27:D30"/>
-    <mergeCell ref="F24:S24"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="F25:S25"/>
-    <mergeCell ref="F26:S26"/>
-    <mergeCell ref="V7:AA7"/>
-    <mergeCell ref="F21:S21"/>
-    <mergeCell ref="F22:S22"/>
-    <mergeCell ref="F16:S16"/>
-    <mergeCell ref="F17:S17"/>
-    <mergeCell ref="F18:S18"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="X8:Y8"/>
-    <mergeCell ref="Z8:AA8"/>
-    <mergeCell ref="Z19:AA27"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="C12:S12"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="C13:S13"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="C15:D18"/>
-    <mergeCell ref="C14:D14"/>
+  <mergeCells count="103">
+    <mergeCell ref="M67:V67"/>
+    <mergeCell ref="M62:V62"/>
+    <mergeCell ref="M63:V63"/>
+    <mergeCell ref="M64:V64"/>
+    <mergeCell ref="M65:V65"/>
+    <mergeCell ref="M66:V66"/>
+    <mergeCell ref="M59:Q59"/>
+    <mergeCell ref="R59:V59"/>
+    <mergeCell ref="M60:Q60"/>
+    <mergeCell ref="R60:V60"/>
+    <mergeCell ref="M61:V61"/>
+    <mergeCell ref="M56:Q56"/>
+    <mergeCell ref="R56:V56"/>
+    <mergeCell ref="M57:Q57"/>
+    <mergeCell ref="R57:V57"/>
+    <mergeCell ref="M58:Q58"/>
+    <mergeCell ref="R58:V58"/>
+    <mergeCell ref="M52:V52"/>
+    <mergeCell ref="M53:V53"/>
+    <mergeCell ref="M54:Q54"/>
+    <mergeCell ref="R54:V54"/>
+    <mergeCell ref="M55:Q55"/>
+    <mergeCell ref="R55:V55"/>
     <mergeCell ref="C31:S31"/>
     <mergeCell ref="C38:G38"/>
     <mergeCell ref="C39:G39"/>
@@ -3244,6 +3415,70 @@
     <mergeCell ref="C19:D22"/>
     <mergeCell ref="F28:S28"/>
     <mergeCell ref="F20:S20"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="C12:S12"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="C13:S13"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="C15:D18"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="V7:AA7"/>
+    <mergeCell ref="F21:S21"/>
+    <mergeCell ref="F22:S22"/>
+    <mergeCell ref="F16:S16"/>
+    <mergeCell ref="F17:S17"/>
+    <mergeCell ref="F18:S18"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="X8:Y8"/>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="Z19:AA27"/>
+    <mergeCell ref="F29:S29"/>
+    <mergeCell ref="F30:S30"/>
+    <mergeCell ref="C23:D26"/>
+    <mergeCell ref="C27:D30"/>
+    <mergeCell ref="F24:S24"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="F25:S25"/>
+    <mergeCell ref="F26:S26"/>
+    <mergeCell ref="C64:L64"/>
+    <mergeCell ref="C65:L65"/>
+    <mergeCell ref="C66:L66"/>
+    <mergeCell ref="C67:L67"/>
+    <mergeCell ref="C59:G59"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="H59:L59"/>
+    <mergeCell ref="H60:L60"/>
+    <mergeCell ref="C52:L52"/>
+    <mergeCell ref="C53:L53"/>
+    <mergeCell ref="C61:L61"/>
+    <mergeCell ref="C62:L62"/>
+    <mergeCell ref="C63:L63"/>
+    <mergeCell ref="H54:L54"/>
+    <mergeCell ref="H55:L55"/>
+    <mergeCell ref="H56:L56"/>
+    <mergeCell ref="H57:L57"/>
+    <mergeCell ref="H58:L58"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="C55:G55"/>
+    <mergeCell ref="C56:G56"/>
+    <mergeCell ref="C57:G57"/>
+    <mergeCell ref="C58:G58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>